<commit_message>
ajout completion date 517ac67fff2b3a09333b9e8c85a6711324c92f04
</commit_message>
<xml_diff>
--- a/ig/sd-add-completion-date/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/sd-add-completion-date/StructureDefinition-eclaire-researchstudy.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$97</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3488" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="613">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-15T14:38:49+00:00</t>
+    <t>2024-01-15T15:20:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1606,6 +1606,65 @@
   </si>
   <si>
     <t>FiveWs.done[x]</t>
+  </si>
+  <si>
+    <t>ResearchStudy.period.id</t>
+  </si>
+  <si>
+    <t>ResearchStudy.period.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.period.start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateTime
+</t>
+  </si>
+  <si>
+    <t>Starting time with inclusive boundary</t>
+  </si>
+  <si>
+    <t>The start of the period. The boundary is inclusive.</t>
+  </si>
+  <si>
+    <t>If the low element is missing, the meaning is that the low boundary is not known.</t>
+  </si>
+  <si>
+    <t>Period.start</t>
+  </si>
+  <si>
+    <t>ele-1
+per-1</t>
+  </si>
+  <si>
+    <t>DR.1</t>
+  </si>
+  <si>
+    <t>./low</t>
+  </si>
+  <si>
+    <t>ResearchStudy.period.end</t>
+  </si>
+  <si>
+    <t>Date à laquelle l'essai se termine (la date initiale est prévisionnelle) / Completion date</t>
+  </si>
+  <si>
+    <t>The end of the period. If the end of the period is missing, it means no end was known or planned at the time the instance was created. The start may be in the past, and the end date in the future, which means that period is expected/planned to end at that time.</t>
+  </si>
+  <si>
+    <t>The high value includes any matching date/time. i.e. 2012-02-03T10:00:00 is in a period that has an end value of 2012-02-03.</t>
+  </si>
+  <si>
+    <t>If the end of the period is missing, it means that the period is ongoing</t>
+  </si>
+  <si>
+    <t>Period.end</t>
+  </si>
+  <si>
+    <t>DR.2</t>
+  </si>
+  <si>
+    <t>./high</t>
   </si>
   <si>
     <t>ResearchStudy.sponsor</t>
@@ -2172,7 +2231,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO93"/>
+  <dimension ref="A1:AO97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -11043,26 +11102,24 @@
         <v>90</v>
       </c>
       <c r="H76" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I76" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>257</v>
+        <v>194</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>514</v>
+        <v>195</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>515</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>287</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="N76" s="2"/>
       <c r="O76" s="2"/>
       <c r="P76" t="s" s="2">
         <v>80</v>
@@ -11111,7 +11168,7 @@
         <v>80</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>513</v>
+        <v>197</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>78</v>
@@ -11120,44 +11177,44 @@
         <v>90</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>262</v>
+        <v>80</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>516</v>
+        <v>80</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>517</v>
+        <v>111</v>
       </c>
       <c r="AN76" t="s" s="2">
-        <v>518</v>
+        <v>80</v>
       </c>
       <c r="AO76" t="s" s="2">
-        <v>519</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>80</v>
@@ -11166,19 +11223,19 @@
         <v>80</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>521</v>
+        <v>138</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>522</v>
+        <v>139</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>523</v>
+        <v>200</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" t="s" s="2">
@@ -11216,54 +11273,54 @@
         <v>80</v>
       </c>
       <c r="AB77" t="s" s="2">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AC77" t="s" s="2">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="AD77" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>520</v>
+        <v>201</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH77" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI77" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>262</v>
+        <v>146</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>524</v>
+        <v>80</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>525</v>
+        <v>104</v>
       </c>
       <c r="AN77" t="s" s="2">
-        <v>526</v>
+        <v>80</v>
       </c>
       <c r="AO77" t="s" s="2">
-        <v>519</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -11274,10 +11331,10 @@
         <v>78</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H78" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I78" t="s" s="2">
         <v>80</v>
@@ -11286,16 +11343,16 @@
         <v>91</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>530</v>
+        <v>518</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>287</v>
+        <v>519</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" t="s" s="2">
@@ -11345,42 +11402,42 @@
         <v>80</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH78" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>102</v>
+        <v>521</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>531</v>
+        <v>80</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>80</v>
+        <v>522</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="AN78" t="s" s="2">
-        <v>532</v>
+        <v>80</v>
       </c>
       <c r="AO78" t="s" s="2">
-        <v>533</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11394,7 +11451,7 @@
         <v>90</v>
       </c>
       <c r="H79" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I79" t="s" s="2">
         <v>80</v>
@@ -11403,22 +11460,24 @@
         <v>91</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>216</v>
+        <v>516</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>310</v>
+        <v>527</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="Q79" s="2"/>
+      <c r="Q79" t="s" s="2">
+        <v>528</v>
+      </c>
       <c r="R79" t="s" s="2">
         <v>80</v>
       </c>
@@ -11438,13 +11497,13 @@
         <v>80</v>
       </c>
       <c r="X79" t="s" s="2">
-        <v>331</v>
+        <v>80</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>537</v>
+        <v>80</v>
       </c>
       <c r="Z79" t="s" s="2">
-        <v>538</v>
+        <v>80</v>
       </c>
       <c r="AA79" t="s" s="2">
         <v>80</v>
@@ -11462,7 +11521,7 @@
         <v>80</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>78</v>
@@ -11471,33 +11530,33 @@
         <v>90</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>102</v>
+        <v>521</v>
       </c>
       <c r="AJ79" t="s" s="2">
         <v>103</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>539</v>
+        <v>80</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>314</v>
+        <v>530</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>315</v>
+        <v>531</v>
       </c>
       <c r="AN79" t="s" s="2">
-        <v>540</v>
+        <v>80</v>
       </c>
       <c r="AO79" t="s" s="2">
-        <v>541</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11508,28 +11567,28 @@
         <v>78</v>
       </c>
       <c r="G80" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H80" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I80" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>543</v>
+        <v>257</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>544</v>
+        <v>533</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="N80" t="s" s="2">
-        <v>546</v>
+        <v>287</v>
       </c>
       <c r="O80" s="2"/>
       <c r="P80" t="s" s="2">
@@ -11579,42 +11638,42 @@
         <v>80</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH80" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI80" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>103</v>
+        <v>262</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>547</v>
+        <v>535</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="AN80" t="s" s="2">
-        <v>80</v>
+        <v>537</v>
       </c>
       <c r="AO80" t="s" s="2">
-        <v>80</v>
+        <v>538</v>
       </c>
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11625,7 +11684,7 @@
         <v>78</v>
       </c>
       <c r="G81" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H81" t="s" s="2">
         <v>80</v>
@@ -11634,18 +11693,20 @@
         <v>80</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>552</v>
-      </c>
-      <c r="N81" s="2"/>
+        <v>542</v>
+      </c>
+      <c r="N81" t="s" s="2">
+        <v>287</v>
+      </c>
       <c r="O81" s="2"/>
       <c r="P81" t="s" s="2">
         <v>80</v>
@@ -11694,42 +11755,42 @@
         <v>80</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="AG81" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI81" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>103</v>
+        <v>262</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="AL81" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM81" t="s" s="2">
-        <v>111</v>
+        <v>544</v>
       </c>
       <c r="AN81" t="s" s="2">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="AO81" t="s" s="2">
-        <v>80</v>
+        <v>538</v>
       </c>
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -11740,27 +11801,29 @@
         <v>78</v>
       </c>
       <c r="G82" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H82" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I82" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>194</v>
+        <v>547</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>195</v>
+        <v>548</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="N82" s="2"/>
+        <v>549</v>
+      </c>
+      <c r="N82" t="s" s="2">
+        <v>287</v>
+      </c>
       <c r="O82" s="2"/>
       <c r="P82" t="s" s="2">
         <v>80</v>
@@ -11809,53 +11872,53 @@
         <v>80</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>197</v>
+        <v>546</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH82" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI82" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AJ82" t="s" s="2">
-        <v>80</v>
+        <v>262</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>80</v>
+        <v>550</v>
       </c>
       <c r="AL82" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>111</v>
+        <v>544</v>
       </c>
       <c r="AN82" t="s" s="2">
-        <v>80</v>
+        <v>551</v>
       </c>
       <c r="AO82" t="s" s="2">
-        <v>80</v>
+        <v>552</v>
       </c>
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G83" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H83" t="s" s="2">
         <v>80</v>
@@ -11864,19 +11927,19 @@
         <v>80</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>138</v>
+        <v>216</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>139</v>
+        <v>554</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>200</v>
+        <v>555</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>141</v>
+        <v>310</v>
       </c>
       <c r="O83" s="2"/>
       <c r="P83" t="s" s="2">
@@ -11902,70 +11965,70 @@
         <v>80</v>
       </c>
       <c r="X83" t="s" s="2">
-        <v>80</v>
+        <v>331</v>
       </c>
       <c r="Y83" t="s" s="2">
-        <v>80</v>
+        <v>556</v>
       </c>
       <c r="Z83" t="s" s="2">
-        <v>80</v>
+        <v>557</v>
       </c>
       <c r="AA83" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AB83" t="s" s="2">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="AC83" t="s" s="2">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="AD83" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>201</v>
+        <v>553</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH83" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI83" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>80</v>
+        <v>558</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>80</v>
+        <v>314</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>104</v>
+        <v>315</v>
       </c>
       <c r="AN83" t="s" s="2">
-        <v>80</v>
+        <v>559</v>
       </c>
       <c r="AO83" t="s" s="2">
-        <v>80</v>
+        <v>560</v>
       </c>
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
-        <v>558</v>
+        <v>80</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
@@ -11978,26 +12041,24 @@
         <v>80</v>
       </c>
       <c r="I84" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>138</v>
+        <v>562</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O84" t="s" s="2">
-        <v>175</v>
-      </c>
+        <v>565</v>
+      </c>
+      <c r="O84" s="2"/>
       <c r="P84" t="s" s="2">
         <v>80</v>
       </c>
@@ -12057,16 +12118,16 @@
         <v>102</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>80</v>
+        <v>566</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>104</v>
+        <v>567</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>80</v>
@@ -12077,10 +12138,10 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12088,10 +12149,10 @@
       </c>
       <c r="E85" s="2"/>
       <c r="F85" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G85" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H85" t="s" s="2">
         <v>80</v>
@@ -12103,17 +12164,15 @@
         <v>80</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>194</v>
+        <v>569</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>564</v>
-      </c>
-      <c r="N85" t="s" s="2">
-        <v>280</v>
-      </c>
+        <v>571</v>
+      </c>
+      <c r="N85" s="2"/>
       <c r="O85" s="2"/>
       <c r="P85" t="s" s="2">
         <v>80</v>
@@ -12162,13 +12221,13 @@
         <v>80</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH85" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI85" t="s" s="2">
         <v>102</v>
@@ -12177,7 +12236,7 @@
         <v>103</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="AL85" t="s" s="2">
         <v>80</v>
@@ -12186,7 +12245,7 @@
         <v>111</v>
       </c>
       <c r="AN85" t="s" s="2">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="AO85" t="s" s="2">
         <v>80</v>
@@ -12194,10 +12253,10 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12220,17 +12279,15 @@
         <v>80</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>568</v>
+        <v>195</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>569</v>
-      </c>
-      <c r="N86" t="s" s="2">
-        <v>310</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="N86" s="2"/>
       <c r="O86" s="2"/>
       <c r="P86" t="s" s="2">
         <v>80</v>
@@ -12279,7 +12336,7 @@
         <v>80</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>567</v>
+        <v>197</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>78</v>
@@ -12288,22 +12345,22 @@
         <v>90</v>
       </c>
       <c r="AI86" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AJ86" t="s" s="2">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="AK86" t="s" s="2">
-        <v>570</v>
+        <v>80</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>314</v>
+        <v>80</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="AN86" t="s" s="2">
-        <v>571</v>
+        <v>80</v>
       </c>
       <c r="AO86" t="s" s="2">
         <v>80</v>
@@ -12311,21 +12368,21 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G87" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H87" t="s" s="2">
         <v>80</v>
@@ -12337,16 +12394,16 @@
         <v>80</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>573</v>
+        <v>139</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>574</v>
+        <v>200</v>
       </c>
       <c r="N87" t="s" s="2">
-        <v>280</v>
+        <v>141</v>
       </c>
       <c r="O87" s="2"/>
       <c r="P87" t="s" s="2">
@@ -12384,43 +12441,43 @@
         <v>80</v>
       </c>
       <c r="AB87" t="s" s="2">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AC87" t="s" s="2">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="AD87" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>572</v>
+        <v>201</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH87" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI87" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="AK87" t="s" s="2">
-        <v>575</v>
+        <v>80</v>
       </c>
       <c r="AL87" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM87" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AN87" t="s" s="2">
-        <v>576</v>
+        <v>80</v>
       </c>
       <c r="AO87" t="s" s="2">
         <v>80</v>
@@ -12428,14 +12485,14 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
-        <v>80</v>
+        <v>577</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" t="s" s="2">
@@ -12448,13 +12505,13 @@
         <v>80</v>
       </c>
       <c r="I88" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J88" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>550</v>
+        <v>138</v>
       </c>
       <c r="L88" t="s" s="2">
         <v>578</v>
@@ -12462,8 +12519,12 @@
       <c r="M88" t="s" s="2">
         <v>579</v>
       </c>
-      <c r="N88" s="2"/>
-      <c r="O88" s="2"/>
+      <c r="N88" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="O88" t="s" s="2">
+        <v>175</v>
+      </c>
       <c r="P88" t="s" s="2">
         <v>80</v>
       </c>
@@ -12511,7 +12572,7 @@
         <v>80</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>78</v>
@@ -12523,16 +12584,16 @@
         <v>102</v>
       </c>
       <c r="AJ88" t="s" s="2">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="AK88" t="s" s="2">
-        <v>580</v>
+        <v>80</v>
       </c>
       <c r="AL88" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AN88" t="s" s="2">
         <v>80</v>
@@ -12554,7 +12615,7 @@
       </c>
       <c r="E89" s="2"/>
       <c r="F89" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G89" t="s" s="2">
         <v>90</v>
@@ -12572,12 +12633,14 @@
         <v>194</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>195</v>
+        <v>582</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="N89" s="2"/>
+        <v>583</v>
+      </c>
+      <c r="N89" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="O89" s="2"/>
       <c r="P89" t="s" s="2">
         <v>80</v>
@@ -12626,22 +12689,22 @@
         <v>80</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>197</v>
+        <v>581</v>
       </c>
       <c r="AG89" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH89" t="s" s="2">
         <v>90</v>
       </c>
       <c r="AI89" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AJ89" t="s" s="2">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="AK89" t="s" s="2">
-        <v>80</v>
+        <v>584</v>
       </c>
       <c r="AL89" t="s" s="2">
         <v>80</v>
@@ -12650,7 +12713,7 @@
         <v>111</v>
       </c>
       <c r="AN89" t="s" s="2">
-        <v>80</v>
+        <v>585</v>
       </c>
       <c r="AO89" t="s" s="2">
         <v>80</v>
@@ -12658,21 +12721,21 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G90" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H90" t="s" s="2">
         <v>80</v>
@@ -12684,16 +12747,16 @@
         <v>80</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>138</v>
+        <v>216</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>139</v>
+        <v>587</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>200</v>
+        <v>588</v>
       </c>
       <c r="N90" t="s" s="2">
-        <v>141</v>
+        <v>310</v>
       </c>
       <c r="O90" s="2"/>
       <c r="P90" t="s" s="2">
@@ -12731,43 +12794,43 @@
         <v>80</v>
       </c>
       <c r="AB90" t="s" s="2">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="AC90" t="s" s="2">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="AD90" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>201</v>
+        <v>586</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH90" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI90" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ90" t="s" s="2">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="AK90" t="s" s="2">
-        <v>80</v>
+        <v>589</v>
       </c>
       <c r="AL90" t="s" s="2">
-        <v>80</v>
+        <v>314</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>104</v>
+        <v>315</v>
       </c>
       <c r="AN90" t="s" s="2">
-        <v>80</v>
+        <v>590</v>
       </c>
       <c r="AO90" t="s" s="2">
         <v>80</v>
@@ -12775,46 +12838,44 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
-        <v>558</v>
+        <v>80</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G91" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H91" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I91" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>138</v>
+        <v>194</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>559</v>
+        <v>592</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>560</v>
+        <v>593</v>
       </c>
       <c r="N91" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O91" t="s" s="2">
-        <v>175</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="O91" s="2"/>
       <c r="P91" t="s" s="2">
         <v>80</v>
       </c>
@@ -12862,31 +12923,31 @@
         <v>80</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>561</v>
+        <v>591</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH91" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI91" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ91" t="s" s="2">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="AK91" t="s" s="2">
-        <v>80</v>
+        <v>594</v>
       </c>
       <c r="AL91" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="AN91" t="s" s="2">
-        <v>80</v>
+        <v>595</v>
       </c>
       <c r="AO91" t="s" s="2">
         <v>80</v>
@@ -12894,10 +12955,10 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
@@ -12908,7 +12969,7 @@
         <v>78</v>
       </c>
       <c r="G92" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H92" t="s" s="2">
         <v>80</v>
@@ -12920,17 +12981,15 @@
         <v>80</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>194</v>
+        <v>569</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>585</v>
+        <v>597</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>586</v>
-      </c>
-      <c r="N92" t="s" s="2">
-        <v>280</v>
-      </c>
+        <v>598</v>
+      </c>
+      <c r="N92" s="2"/>
       <c r="O92" s="2"/>
       <c r="P92" t="s" s="2">
         <v>80</v>
@@ -12979,13 +13038,13 @@
         <v>80</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH92" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI92" t="s" s="2">
         <v>102</v>
@@ -12994,7 +13053,7 @@
         <v>103</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>587</v>
+        <v>599</v>
       </c>
       <c r="AL92" t="s" s="2">
         <v>80</v>
@@ -13011,10 +13070,10 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>588</v>
+        <v>600</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>588</v>
+        <v>600</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -13037,17 +13096,15 @@
         <v>80</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>589</v>
+        <v>195</v>
       </c>
       <c r="M93" t="s" s="2">
-        <v>590</v>
-      </c>
-      <c r="N93" t="s" s="2">
-        <v>310</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="N93" s="2"/>
       <c r="O93" s="2"/>
       <c r="P93" t="s" s="2">
         <v>80</v>
@@ -13072,13 +13129,13 @@
         <v>80</v>
       </c>
       <c r="X93" t="s" s="2">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="Y93" t="s" s="2">
-        <v>591</v>
+        <v>80</v>
       </c>
       <c r="Z93" t="s" s="2">
-        <v>592</v>
+        <v>80</v>
       </c>
       <c r="AA93" t="s" s="2">
         <v>80</v>
@@ -13096,7 +13153,7 @@
         <v>80</v>
       </c>
       <c r="AF93" t="s" s="2">
-        <v>588</v>
+        <v>197</v>
       </c>
       <c r="AG93" t="s" s="2">
         <v>78</v>
@@ -13105,29 +13162,499 @@
         <v>90</v>
       </c>
       <c r="AI93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM93" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AN93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO93" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" hidden="true">
+      <c r="A94" t="s" s="2">
+        <v>601</v>
+      </c>
+      <c r="B94" t="s" s="2">
+        <v>601</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G94" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K94" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="L94" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="M94" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="N94" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="O94" s="2"/>
+      <c r="P94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q94" s="2"/>
+      <c r="R94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB94" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AC94" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="AD94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE94" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="AF94" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="AG94" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH94" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI94" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="AJ93" t="s" s="2">
+      <c r="AJ94" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="AK94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM94" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AN94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO94" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="95" hidden="true">
+      <c r="A95" t="s" s="2">
+        <v>602</v>
+      </c>
+      <c r="B95" t="s" s="2">
+        <v>602</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" t="s" s="2">
+        <v>577</v>
+      </c>
+      <c r="E95" s="2"/>
+      <c r="F95" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G95" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I95" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="J95" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K95" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="L95" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="M95" t="s" s="2">
+        <v>579</v>
+      </c>
+      <c r="N95" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="O95" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="P95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q95" s="2"/>
+      <c r="R95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF95" t="s" s="2">
+        <v>580</v>
+      </c>
+      <c r="AG95" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH95" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI95" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ95" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="AK95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM95" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AN95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO95" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" hidden="true">
+      <c r="A96" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="B96" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E96" s="2"/>
+      <c r="F96" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G96" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="H96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K96" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="L96" t="s" s="2">
+        <v>604</v>
+      </c>
+      <c r="M96" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="N96" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="O96" s="2"/>
+      <c r="P96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q96" s="2"/>
+      <c r="R96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="AK93" t="s" s="2">
-        <v>593</v>
-      </c>
-      <c r="AL93" t="s" s="2">
+      <c r="AK96" t="s" s="2">
+        <v>606</v>
+      </c>
+      <c r="AL96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM96" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AN96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO96" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" hidden="true">
+      <c r="A97" t="s" s="2">
+        <v>607</v>
+      </c>
+      <c r="B97" t="s" s="2">
+        <v>607</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E97" s="2"/>
+      <c r="F97" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G97" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="H97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K97" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L97" t="s" s="2">
+        <v>608</v>
+      </c>
+      <c r="M97" t="s" s="2">
+        <v>609</v>
+      </c>
+      <c r="N97" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="O97" s="2"/>
+      <c r="P97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q97" s="2"/>
+      <c r="R97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X97" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="Y97" t="s" s="2">
+        <v>610</v>
+      </c>
+      <c r="Z97" t="s" s="2">
+        <v>611</v>
+      </c>
+      <c r="AA97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF97" t="s" s="2">
+        <v>607</v>
+      </c>
+      <c r="AG97" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH97" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AI97" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ97" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK97" t="s" s="2">
+        <v>612</v>
+      </c>
+      <c r="AL97" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="AM93" t="s" s="2">
+      <c r="AM97" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="AN93" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AO93" t="s" s="2">
+      <c r="AN97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO97" t="s" s="2">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO93">
+  <autoFilter ref="A1:AO97">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -13137,7 +13664,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI92">
+  <conditionalFormatting sqref="A2:AI96">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>